<commit_message>
Update bot.py + fix coordonate Linella si CIP
</commit_message>
<xml_diff>
--- a/data/linella_google_full.xlsx
+++ b/data/linella_google_full.xlsx
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,10 +1268,10 @@
         <v>20</v>
       </c>
       <c r="J6">
-        <v>47.036535099999988</v>
+        <v>47.0353984666747</v>
       </c>
       <c r="K6">
-        <v>28.777653999999991</v>
+        <v>28.776644048563298</v>
       </c>
       <c r="M6" t="s">
         <v>15</v>
@@ -2864,10 +2864,10 @@
         <v>20</v>
       </c>
       <c r="J48">
-        <v>47.021674999999988</v>
+        <v>47.021821000000003</v>
       </c>
       <c r="K48">
-        <v>28.8010096</v>
+        <v>28.799395000000001</v>
       </c>
       <c r="M48" t="s">
         <v>15</v>
@@ -7897,10 +7897,10 @@
         <v>20</v>
       </c>
       <c r="J181">
-        <v>47.740817799999988</v>
+        <v>47.7504231648089</v>
       </c>
       <c r="K181">
-        <v>27.8761774</v>
+        <v>27.901553753894699</v>
       </c>
       <c r="M181" t="s">
         <v>15</v>
@@ -8429,10 +8429,10 @@
         <v>20</v>
       </c>
       <c r="J195">
-        <v>47.740817799999988</v>
+        <v>47.740960827715803</v>
       </c>
       <c r="K195">
-        <v>27.8761774</v>
+        <v>27.877507350726201</v>
       </c>
       <c r="M195" t="s">
         <v>15</v>

</xml_diff>